<commit_message>
agora com umidade na planilha 2
</commit_message>
<xml_diff>
--- a/Código de cores/arqcomp sprint 2 graficos fases1-3.xlsx
+++ b/Código de cores/arqcomp sprint 2 graficos fases1-3.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14130" windowHeight="4560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14130" windowHeight="4560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>abaixo do limite</t>
   </si>
@@ -100,6 +101,27 @@
   <si>
     <t>holder</t>
   </si>
+  <si>
+    <t>Umidade máxima</t>
+  </si>
+  <si>
+    <t>Umidade mínima</t>
+  </si>
+  <si>
+    <t>Alerta (muito umido)</t>
+  </si>
+  <si>
+    <t>Alerta (muito seco)</t>
+  </si>
+  <si>
+    <t>Umidade:</t>
+  </si>
+  <si>
+    <t>muito seco</t>
+  </si>
+  <si>
+    <t>muito umido</t>
+  </si>
 </sst>
 </file>
 
@@ -164,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -182,6 +204,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2995,6 +3034,925 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Umidade</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha2!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Umidade máxima</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha2!$D$4:$J$4</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8A80-4E74-B056-48E351AAE3F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha2!$C$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Alerta (muito umido)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha2!$D$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8A80-4E74-B056-48E351AAE3F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha2!$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dado (temperatura)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha2!$D$6:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.73</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8A80-4E74-B056-48E351AAE3F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha2!$C$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Alerta (muito seco)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha2!$D$7:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8A80-4E74-B056-48E351AAE3F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha2!$C$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Umidade mínima</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha2!$D$8:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8A80-4E74-B056-48E351AAE3F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1034285183"/>
+        <c:axId val="1091705551"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1034285183"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1091705551"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1091705551"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="95000"/>
+                      <a:lumOff val="5000"/>
+                      <a:alpha val="42000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                      <a:alpha val="36000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1034285183"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3115,6 +4073,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="228">
   <cs:axisTitle>
@@ -4252,6 +5250,574 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="228">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="17"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="228">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4906,6 +6472,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5179,8 +6780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AG50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AG44" sqref="AG44"/>
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5887,4 +7488,186 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:Q8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="G4" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="I4" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="J4" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="G5" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="I5" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="J5" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="M5" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="N5" s="8">
+        <v>0.65</v>
+      </c>
+      <c r="O5" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="P5" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="Q5" s="11">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0.71</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.65</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0.62</v>
+      </c>
+      <c r="G6" s="13">
+        <v>0.66</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0.76</v>
+      </c>
+      <c r="I6" s="13">
+        <v>0.74</v>
+      </c>
+      <c r="J6" s="13">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0.65</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0.65</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0.65</v>
+      </c>
+      <c r="G7" s="13">
+        <v>0.65</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0.65</v>
+      </c>
+      <c r="I7" s="13">
+        <v>0.65</v>
+      </c>
+      <c r="J7" s="13">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0.6</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0.6</v>
+      </c>
+      <c r="F8" s="13">
+        <v>0.6</v>
+      </c>
+      <c r="G8" s="13">
+        <v>0.6</v>
+      </c>
+      <c r="H8" s="13">
+        <v>0.6</v>
+      </c>
+      <c r="I8" s="13">
+        <v>0.6</v>
+      </c>
+      <c r="J8" s="13">
+        <v>0.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>